<commit_message>
Build site at 2025-03-12 13:25:14 UTC
</commit_message>
<xml_diff>
--- a/_Drive/Publicacoes/baptista.xlsx
+++ b/_Drive/Publicacoes/baptista.xlsx
@@ -8,167 +8,548 @@
   <definedNames/>
   <calcPr/>
   <extLst>
-    <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mh2F+sBrPkGL4ebfe9JBs6w/c3dSQ=="/>
+    <ext uri="GoogleSheetsCustomDataVersion2">
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="R10F2LvE1O3Bfdnfxd9rkr+BTeGxJzAVxU/y8rgrfdA="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
   <si>
     <t>DOI</t>
   </si>
   <si>
-    <t>10.1016/j.ijfatigue.2016.04.018</t>
-  </si>
-  <si>
-    <t>10.1016/j.proeng.2010.03.178</t>
-  </si>
-  <si>
-    <t>10.1016/j.engfailanal.2006.11.053</t>
-  </si>
-  <si>
-    <t>10.1007/s40430-019-1821-9</t>
-  </si>
-  <si>
-    <t>10.1016/j.prostr.2019.08.054</t>
-  </si>
-  <si>
-    <t>10.4028/www.scientific.net/amr.1135.167</t>
-  </si>
-  <si>
-    <t>10.17563/rbav.v34i1.939</t>
-  </si>
-  <si>
-    <t>10.1243/14644207JMDA122</t>
-  </si>
-  <si>
-    <t>10.20906/CPS/COB-2015-1461</t>
-  </si>
-  <si>
-    <t>10.1016/j.proeng.2010.03.205</t>
-  </si>
-  <si>
-    <t>10.20906/CPS/COB-2015-0858</t>
-  </si>
-  <si>
-    <t>10.4028/www.scientific.net/msf.805.204</t>
-  </si>
-  <si>
-    <t>10.1590/0370-44672019740154</t>
-  </si>
-  <si>
-    <t>10.4028/www.scientific.net/KEM.713.30</t>
-  </si>
-  <si>
-    <t>10.1016/j.ceramint.2012.08.093</t>
-  </si>
-  <si>
-    <t>10.1016/j.proeng.2011.04.342</t>
-  </si>
-  <si>
-    <t>10.4028/www.scientific.net/AMR.891-892.615</t>
-  </si>
-  <si>
-    <t>10.1007/s40430-014-0175-6</t>
-  </si>
-  <si>
-    <t>10.1016/j.ijfatigue.2004.01.011</t>
-  </si>
-  <si>
-    <t>10.1016/j.proeng.2011.04.339</t>
-  </si>
-  <si>
-    <t>10.4028/www.scientific.net/AMR.891-892.1507</t>
-  </si>
-  <si>
-    <t>10.4028/www.scientific.net/kem.754.248</t>
-  </si>
-  <si>
-    <t>10.1016/j.proeng.2011.04.343</t>
-  </si>
-  <si>
-    <t>10.5028/jatm.v5i2.219</t>
-  </si>
-  <si>
-    <t>10.1016/j.jmrt.2021.01.038</t>
-  </si>
-  <si>
-    <t>10.1016/j.msea.2006.10.124</t>
-  </si>
-  <si>
-    <t>10.4028/www.scientific.net/AMR.891-892.1335</t>
-  </si>
-  <si>
-    <t>10.17563/rbav.v34i2.956</t>
-  </si>
-  <si>
-    <t>10.1016/j.jmrt.2013.10.005</t>
-  </si>
-  <si>
-    <t>10.3390/met9050589</t>
-  </si>
-  <si>
-    <t>10.4028/www.scientific.net/MSF.727-728.945</t>
-  </si>
-  <si>
-    <t>10.1016/j.matdes.2008.08.010</t>
-  </si>
-  <si>
-    <t>10.1051/matecconf/202032111095</t>
-  </si>
-  <si>
-    <t>10.1016/j.proeng.2011.04.220</t>
-  </si>
-  <si>
-    <t>10.1088/2053-1591/ab6c8f</t>
-  </si>
-  <si>
-    <t>10.4028/www.scientific.net/MSF.636-637.47</t>
-  </si>
-  <si>
-    <t>10.4028/www.scientific.net/kem.754.43</t>
-  </si>
-  <si>
-    <t>10.1590/0370-44672018720157</t>
-  </si>
-  <si>
-    <t>10.1016/j.proeng.2010.03.206</t>
-  </si>
-  <si>
-    <t>10.20906/CPS/COB-2015-0934</t>
-  </si>
-  <si>
-    <t>10.1016/j.mechmat.2012.04.003</t>
-  </si>
-  <si>
-    <t>10.1016/j.jmbbm.2014.06.011</t>
-  </si>
-  <si>
-    <t>10.1590/s0366-69132014000100006</t>
-  </si>
-  <si>
-    <t>10.1177/0021998310376098</t>
-  </si>
-  <si>
-    <t>10.4028/www.scientific.net/AMR.891-892.1785</t>
-  </si>
-  <si>
-    <t>10.1016/j.proeng.2011.04.202</t>
-  </si>
-  <si>
-    <t>10.4028/www.scientific.net/msf.869.503</t>
-  </si>
-  <si>
-    <t>10.1016/j.prostr.2019.08.043</t>
-  </si>
-  <si>
-    <t>10.4028/www.scientific.net/AMR.891-892.1767</t>
-  </si>
-  <si>
-    <t>10.3390/met11122034</t>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>10.1007/s00170-023-12686-2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>10.1007/s11665-022-06795-4</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>10.1007/s40430-014-0175-6</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>10.1007/s40430-019-1821-9</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>10.1007/s40430-023-04540-z</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>10.1007/s40430-024-05069-5</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>10.1007/s42247-024-00746-6</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>10.1016/j.ceramint.2012.08.093</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>10.1016/j.engfailanal.2006.11.053</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>10.1016/j.ijfatigue.2004.01.011</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>10.1016/j.ijfatigue.2016.04.018</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>10.1016/j.jmbbm.2014.06.011</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>10.1016/j.jmrt.2013.10.005</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>10.1016/j.jmrt.2021.01.038</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>10.1016/j.matdes.2008.08.010</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>10.1016/j.mechmat.2012.04.003</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>10.1016/j.msea.2006.10.124</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>10.1016/j.msea.2025.148040</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>10.1016/j.proeng.2010.03.178</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>10.1016/j.proeng.2010.03.205</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>10.1016/j.proeng.2010.03.206</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>10.1016/j.proeng.2011.04.202</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>10.1016/j.proeng.2011.04.220</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>10.1016/j.proeng.2011.04.339</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>10.1016/j.proeng.2011.04.342</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>10.1016/j.proeng.2011.04.343</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>10.1016/j.prostr.2019.08.043</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>10.1016/j.prostr.2019.08.054</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>10.1051/matecconf/202032111095</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>10.1088/2053-1591/ab6c8f</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>10.1177/0021998310376098</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>10.1243/14644207JMDA122</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>10.1590/0366-69132022683863210</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>10.1590/0370-44672018720157</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>10.1590/0370-44672019740154</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>10.1590/1980-5373-MR-2022-0315</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>10.1590/s0366-69132014000100006</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>10.17563/rbav.v34i1.939</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>10.17563/rbav.v34i2.956</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>10.20906/CPS/COB-2015-0858</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>10.20906/CPS/COB-2015-0934</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>10.20906/CPS/COB-2015-1461</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>10.26678/ABCM.COBEM2023.COB2023-0535</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>10.3390/met11122034</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>10.3390/met9050589</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>10.4028/www.scientific.net/AMR.891-892.1335</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>10.4028/www.scientific.net/AMR.891-892.1507</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>10.4028/www.scientific.net/AMR.891-892.1767</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>10.4028/www.scientific.net/AMR.891-892.1785</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>10.4028/www.scientific.net/AMR.891-892.615</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>10.4028/www.scientific.net/KEM.713.30</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>10.4028/www.scientific.net/MSF.636-637.47</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>10.4028/www.scientific.net/MSF.727-728.945</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>10.4028/www.scientific.net/amr.1135.167</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>10.4028/www.scientific.net/kem.754.248</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>10.4028/www.scientific.net/kem.754.43</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>10.4028/www.scientific.net/msf.805.204</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>10.4028/www.scientific.net/msf.869.503</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>10.5028/jatm.v5i2.219</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -179,7 +560,8 @@
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
-      <name val="Sans"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -188,8 +570,8 @@
       <name val="Sans"/>
     </font>
     <font>
-      <color theme="1"/>
-      <name val="Calibri"/>
+      <u/>
+      <color rgb="FF0000FF"/>
     </font>
   </fonts>
   <fills count="2">
@@ -206,14 +588,13 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -689,27 +1070,55 @@
       </c>
     </row>
     <row r="51" ht="12.75" customHeight="1">
-      <c r="A51" s="3" t="s">
-        <v>25</v>
+      <c r="A51" s="2" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="52" ht="12.75" customHeight="1">
-      <c r="A52" s="3" t="s">
-        <v>13</v>
+      <c r="A52" s="2" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="53" ht="12.75" customHeight="1">
-      <c r="A53" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="54" ht="12.75" customHeight="1"/>
-    <row r="55" ht="12.75" customHeight="1"/>
-    <row r="56" ht="12.75" customHeight="1"/>
-    <row r="57" ht="12.75" customHeight="1"/>
-    <row r="58" ht="12.75" customHeight="1"/>
-    <row r="59" ht="12.75" customHeight="1"/>
-    <row r="60" ht="12.75" customHeight="1"/>
+      <c r="A53" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" ht="12.75" customHeight="1">
+      <c r="A54" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" ht="12.75" customHeight="1">
+      <c r="A55" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" ht="12.75" customHeight="1">
+      <c r="A56" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" ht="12.75" customHeight="1">
+      <c r="A57" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" ht="12.75" customHeight="1">
+      <c r="A58" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" ht="12.75" customHeight="1">
+      <c r="A59" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" ht="12.75" customHeight="1">
+      <c r="A60" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
     <row r="61" ht="12.75" customHeight="1"/>
     <row r="62" ht="12.75" customHeight="1"/>
     <row r="63" ht="12.75" customHeight="1"/>
@@ -1651,6 +2060,67 @@
     <row r="999" ht="12.75" customHeight="1"/>
     <row r="1000" ht="12.75" customHeight="1"/>
   </sheetData>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="A2"/>
+    <hyperlink r:id="rId2" ref="A3"/>
+    <hyperlink r:id="rId3" ref="A4"/>
+    <hyperlink r:id="rId4" ref="A5"/>
+    <hyperlink r:id="rId5" ref="A6"/>
+    <hyperlink r:id="rId6" ref="A7"/>
+    <hyperlink r:id="rId7" ref="A8"/>
+    <hyperlink r:id="rId8" ref="A9"/>
+    <hyperlink r:id="rId9" ref="A10"/>
+    <hyperlink r:id="rId10" ref="A11"/>
+    <hyperlink r:id="rId11" ref="A12"/>
+    <hyperlink r:id="rId12" ref="A13"/>
+    <hyperlink r:id="rId13" ref="A14"/>
+    <hyperlink r:id="rId14" ref="A15"/>
+    <hyperlink r:id="rId15" ref="A16"/>
+    <hyperlink r:id="rId16" ref="A17"/>
+    <hyperlink r:id="rId17" ref="A18"/>
+    <hyperlink r:id="rId18" ref="A19"/>
+    <hyperlink r:id="rId19" ref="A20"/>
+    <hyperlink r:id="rId20" ref="A21"/>
+    <hyperlink r:id="rId21" ref="A22"/>
+    <hyperlink r:id="rId22" ref="A23"/>
+    <hyperlink r:id="rId23" ref="A24"/>
+    <hyperlink r:id="rId24" ref="A25"/>
+    <hyperlink r:id="rId25" ref="A26"/>
+    <hyperlink r:id="rId26" ref="A27"/>
+    <hyperlink r:id="rId27" ref="A28"/>
+    <hyperlink r:id="rId28" ref="A29"/>
+    <hyperlink r:id="rId29" ref="A30"/>
+    <hyperlink r:id="rId30" ref="A31"/>
+    <hyperlink r:id="rId31" ref="A32"/>
+    <hyperlink r:id="rId32" ref="A33"/>
+    <hyperlink r:id="rId33" ref="A34"/>
+    <hyperlink r:id="rId34" ref="A35"/>
+    <hyperlink r:id="rId35" ref="A36"/>
+    <hyperlink r:id="rId36" ref="A37"/>
+    <hyperlink r:id="rId37" ref="A38"/>
+    <hyperlink r:id="rId38" ref="A39"/>
+    <hyperlink r:id="rId39" ref="A40"/>
+    <hyperlink r:id="rId40" ref="A41"/>
+    <hyperlink r:id="rId41" ref="A42"/>
+    <hyperlink r:id="rId42" ref="A43"/>
+    <hyperlink r:id="rId43" ref="A44"/>
+    <hyperlink r:id="rId44" ref="A45"/>
+    <hyperlink r:id="rId45" ref="A46"/>
+    <hyperlink r:id="rId46" ref="A47"/>
+    <hyperlink r:id="rId47" ref="A48"/>
+    <hyperlink r:id="rId48" ref="A49"/>
+    <hyperlink r:id="rId49" ref="A50"/>
+    <hyperlink r:id="rId50" ref="A51"/>
+    <hyperlink r:id="rId51" ref="A52"/>
+    <hyperlink r:id="rId52" ref="A53"/>
+    <hyperlink r:id="rId53" ref="A54"/>
+    <hyperlink r:id="rId54" ref="A55"/>
+    <hyperlink r:id="rId55" ref="A56"/>
+    <hyperlink r:id="rId56" ref="A57"/>
+    <hyperlink r:id="rId57" ref="A58"/>
+    <hyperlink r:id="rId58" ref="A59"/>
+    <hyperlink r:id="rId59" ref="A60"/>
+  </hyperlinks>
   <printOptions/>
   <pageMargins bottom="1.6666666666666667" footer="0.0" header="0.0" left="1.0" right="1.0" top="1.6666666666666667"/>
   <pageSetup paperSize="9" cellComments="atEnd" orientation="portrait"/>
@@ -1658,6 +2128,6 @@
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId60"/>
 </worksheet>
 </file>
</xml_diff>